<commit_message>
fix: update family budget spreadsheet with latest changes
Updated the "Family budget monthly.xlsx" file to reflect recent adjustments. This ensures the data remains accurate and up-to-date.
</commit_message>
<xml_diff>
--- a/spreadsheets/Family budget monthly.xlsx
+++ b/spreadsheets/Family budget monthly.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBD0D0F-A8C5-4C7E-BA7E-0FC6312BDFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D845729B-985F-47B1-8204-AE02E860C512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6430" yWindow="2970" windowWidth="25700" windowHeight="14450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly budget report" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Savings" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses1" hidden="1">TBL_MonthlyExpenses[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses" hidden="1">TBL_MonthlyExpenses[]</definedName>
     <definedName name="List_ExpenseCategories">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Monthly expenses'!$2:$4</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="TBL_MonthlyExpenses" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -367,7 +367,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0_);[Red]\(&quot;$&quot;\ #,##0\)"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;\ #,##0.0000_);[Red]\(&quot;$&quot;\ #,##0.0000\)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.0000_);[Red]\(&quot;$&quot;\ #,##0.0000\)"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -833,6 +833,27 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -841,27 +862,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1592,16 +1592,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>336176</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1139265</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>321210</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>57982</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>172854</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>217907</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1629,8 +1629,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10944411" y="1602441"/>
-          <a:ext cx="4053363" cy="3087398"/>
+          <a:off x="9521239" y="319875"/>
+          <a:ext cx="4098903" cy="3092840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1882,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1922,12 +1922,12 @@
     <row r="3" spans="1:12" s="3" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="1.85">
       <c r="A3" s="10"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1959,11 +1959,11 @@
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
     </row>
@@ -1981,11 +1981,11 @@
         <v>4</v>
       </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="69" t="s">
+      <c r="H6" s="64"/>
+      <c r="I6" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="66" t="s">
         <v>87</v>
       </c>
       <c r="K6" s="14"/>
@@ -2010,14 +2010,14 @@
         <v>155</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="65">
         <f>Savings!F65</f>
         <v>41911.804008200437</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="69">
         <f>Savings!D65</f>
         <v>51.700129847940623</v>
       </c>
@@ -2043,9 +2043,9 @@
         <v>-55</v>
       </c>
       <c r="G8" s="14"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
       <c r="K8" s="8"/>
       <c r="L8" s="14"/>
     </row>
@@ -2367,8 +2367,8 @@
   </sheetPr>
   <dimension ref="B1:H69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CZ196" sqref="CZ196"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2384,11 +2384,11 @@
     <row r="1" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:8" s="7" customFormat="1" ht="80.05" customHeight="1" thickTop="1" x14ac:dyDescent="1.85">
       <c r="B2" s="29"/>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
       <c r="H2" s="29"/>
@@ -4816,35 +4816,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5144,27 +5115,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AB306A1-AFF6-40CB-BF3D-1EF22BB7168E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5185,6 +5165,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
feat: add area detection for spreadsheet analysis
Implemented `DetectAreas` pass to identify connected cell regions in spreadsheets. Added `Area` record, helper functions, and integrated logic into the conversion process. This improves structural analysis by grouping related cell regions effectively.
</commit_message>
<xml_diff>
--- a/spreadsheets/Family budget monthly.xlsx
+++ b/spreadsheets/Family budget monthly.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D845729B-985F-47B1-8204-AE02E860C512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35C3E1D-0E4D-42AD-BCA1-842F43FAA3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly budget report" sheetId="2" r:id="rId1"/>
     <sheet name="Monthly expenses" sheetId="3" r:id="rId2"/>
-    <sheet name="Savings" sheetId="6" r:id="rId3"/>
+    <sheet name="Interest" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses" hidden="1">TBL_MonthlyExpenses[]</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>Savings Account 1</t>
+  </si>
+  <si>
+    <t>Test?!</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -619,37 +622,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF00682F"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF00682F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF00682F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF00682F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF00682F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -663,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -824,13 +796,10 @@
     <xf numFmtId="49" fontId="22" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1658,15 +1627,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{46B4E492-9B14-4202-8E51-42A2EDF52486}" name="Table2" displayName="Table2" ref="C4:F65" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="C4:F65" xr:uid="{46B4E492-9B14-4202-8E51-42A2EDF52486}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9D1C6E41-060D-4F97-BF77-7C8F09BCC41D}" name="Table24" displayName="Table24" ref="C4:F65" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="C4:F65" xr:uid="{9D1C6E41-060D-4F97-BF77-7C8F09BCC41D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60D90F81-A33C-4DBA-960C-192DF1442412}" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{9F6832B8-C2BC-4608-BCA0-3354D3D2FE4F}" name="Interest" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{3D59A9F2-EF62-4C23-9106-2C299EB960F7}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{54AB7298-BD13-4A9A-8553-DC2A3ED98DEE}" name="Interest" dataDxfId="4">
       <calculatedColumnFormula>$J$9*F4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{221E450F-4216-439A-A37E-28D8055CEE6F}" name="Deposit" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2BADD937-4897-443E-A711-FB841CD338A2}" name="Total" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{955807F8-4A68-4CDC-A24B-36FE09F729AA}" name="Deposit" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{4294E201-A994-47DC-9E73-CB4A3A2683F5}" name="Total" dataDxfId="2">
       <calculatedColumnFormula>F4+D5+E5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1882,8 +1851,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1894,7 +1863,7 @@
     <col min="7" max="7" width="2.59765625" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.19921875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.59765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.265625" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.1328125" style="1" customWidth="1"/>
     <col min="12" max="12" width="2.59765625" style="1" customWidth="1"/>
     <col min="13" max="16" width="8.86328125" style="1" customWidth="1"/>
@@ -1922,12 +1891,12 @@
     <row r="3" spans="1:12" s="3" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="1.85">
       <c r="A3" s="10"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1959,11 +1928,11 @@
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
     </row>
@@ -1981,11 +1950,11 @@
         <v>4</v>
       </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="66" t="s">
+      <c r="H6" s="61"/>
+      <c r="I6" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="66" t="s">
+      <c r="J6" s="63" t="s">
         <v>87</v>
       </c>
       <c r="K6" s="14"/>
@@ -1999,27 +1968,27 @@
       </c>
       <c r="D7" s="23">
         <f>D9+D10-D8</f>
-        <v>1636.7001298479408</v>
+        <v>3496.8040082004372</v>
       </c>
       <c r="E7" s="23">
         <f>E9+E10-E8</f>
-        <v>1791.7001298479408</v>
+        <v>3651.8040082004372</v>
       </c>
       <c r="F7" s="24">
         <f>E7-D7</f>
         <v>155</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="67" t="s">
+      <c r="H7" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="I7" s="65">
-        <f>Savings!F65</f>
+      <c r="I7" s="62">
+        <f>Interest!F65</f>
         <v>41911.804008200437</v>
       </c>
-      <c r="J7" s="69">
-        <f>Savings!D65</f>
-        <v>51.700129847940623</v>
+      <c r="J7" s="66">
+        <f>Interest!J12</f>
+        <v>1911.8040082004372</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
@@ -2043,9 +2012,9 @@
         <v>-55</v>
       </c>
       <c r="G8" s="14"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="8"/>
       <c r="L8" s="14"/>
     </row>
@@ -2082,11 +2051,11 @@
       </c>
       <c r="D10" s="23">
         <f>$J7</f>
-        <v>51.700129847940623</v>
+        <v>1911.8040082004372</v>
       </c>
       <c r="E10" s="23">
         <f>$J7</f>
-        <v>51.700129847940623</v>
+        <v>1911.8040082004372</v>
       </c>
       <c r="F10" s="24">
         <f>E10-D10</f>
@@ -2348,7 +2317,7 @@
   <mergeCells count="1">
     <mergeCell ref="C3:F3"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your projected income in this cell" sqref="D15:D17 I6:I8" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter you actual income in this cell" sqref="E15:E17 J7:J8" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Difference is auto calculated in this cell" sqref="F15:F17" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
@@ -2365,10 +2334,10 @@
     <tabColor theme="8"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H69"/>
+  <dimension ref="B1:M69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2381,19 +2350,19 @@
     <col min="10" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:8" s="7" customFormat="1" ht="80.05" customHeight="1" thickTop="1" x14ac:dyDescent="1.85">
+    <row r="1" spans="2:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:13" s="7" customFormat="1" ht="80.05" customHeight="1" thickTop="1" x14ac:dyDescent="1.85">
       <c r="B2" s="29"/>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
       <c r="H2" s="29"/>
     </row>
-    <row r="3" spans="2:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" ht="20.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="8"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -2402,7 +2371,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="22"/>
       <c r="C4" s="39" t="s">
         <v>9</v>
@@ -2421,7 +2390,7 @@
       </c>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="8"/>
       <c r="C5" s="41" t="s">
         <v>55</v>
@@ -2441,7 +2410,7 @@
       </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="41" t="s">
         <v>12</v>
@@ -2461,7 +2430,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="8"/>
       <c r="C7" s="41" t="s">
         <v>56</v>
@@ -2481,7 +2450,7 @@
       </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="8"/>
       <c r="C8" s="41" t="s">
         <v>57</v>
@@ -2501,7 +2470,7 @@
       </c>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="8"/>
       <c r="C9" s="41" t="s">
         <v>13</v>
@@ -2521,7 +2490,7 @@
       </c>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="8"/>
       <c r="C10" s="41" t="s">
         <v>58</v>
@@ -2541,7 +2510,7 @@
       </c>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="8"/>
       <c r="C11" s="41" t="s">
         <v>15</v>
@@ -2561,7 +2530,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="8"/>
       <c r="C12" s="41" t="s">
         <v>59</v>
@@ -2581,7 +2550,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="8"/>
       <c r="C13" s="41" t="s">
         <v>60</v>
@@ -2601,7 +2570,7 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="8"/>
       <c r="C14" s="41" t="s">
         <v>61</v>
@@ -2620,8 +2589,11 @@
         <v>-30</v>
       </c>
       <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M14" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="8"/>
       <c r="C15" s="41" t="s">
         <v>62</v>
@@ -2641,7 +2613,7 @@
       </c>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="8"/>
       <c r="C16" s="41" t="s">
         <v>63</v>
@@ -3593,45 +3565,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6496504D-7C5D-4BE8-BC8D-E626AF5EB2CE}">
-  <sheetPr codeName="Sheet5">
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B618A38-7516-49C0-AD89-7C048EC36DD6}">
   <dimension ref="B1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.53125" customWidth="1"/>
-    <col min="2" max="2" width="3.265625" customWidth="1"/>
-    <col min="3" max="3" width="17.73046875" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="5" max="5" width="16.06640625" customWidth="1"/>
-    <col min="6" max="6" width="19.796875" customWidth="1"/>
-    <col min="7" max="7" width="4.1328125" customWidth="1"/>
-    <col min="9" max="9" width="19.3984375" customWidth="1"/>
+    <col min="9" max="9" width="20.73046875" customWidth="1"/>
+    <col min="10" max="10" width="13.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="58"/>
-    </row>
-    <row r="2" spans="2:10" ht="78" customHeight="1" thickTop="1" x14ac:dyDescent="1.85">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
+    <row r="1" spans="2:10" ht="15.45" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" ht="66.45" thickTop="1" x14ac:dyDescent="1.85">
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B3" s="51"/>
@@ -3641,7 +3597,7 @@
       <c r="F3" s="53"/>
       <c r="G3" s="51"/>
     </row>
-    <row r="4" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" ht="17.600000000000001" x14ac:dyDescent="0.45">
       <c r="B4" s="51"/>
       <c r="C4" s="55" t="s">
         <v>86</v>
@@ -3657,7 +3613,7 @@
       </c>
       <c r="G4" s="51"/>
     </row>
-    <row r="5" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" ht="35.15" x14ac:dyDescent="0.45">
       <c r="B5" s="51"/>
       <c r="C5" s="49">
         <v>44256</v>
@@ -3673,13 +3629,13 @@
       </c>
       <c r="J5" s="45"/>
     </row>
-    <row r="6" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" ht="35.15" x14ac:dyDescent="0.45">
       <c r="B6" s="51"/>
       <c r="C6" s="49">
         <v>44287</v>
       </c>
       <c r="D6" s="50">
-        <f t="shared" ref="D6:D37" si="0">$J$9*F5</f>
+        <f t="shared" ref="D6:D65" si="0">$J$9*F5</f>
         <v>12.5</v>
       </c>
       <c r="E6" s="50">
@@ -3697,7 +3653,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" ht="17.600000000000001" x14ac:dyDescent="0.45">
       <c r="B7" s="51"/>
       <c r="C7" s="49">
         <v>44317</v>
@@ -3710,13 +3666,13 @@
         <v>500</v>
       </c>
       <c r="F7" s="50">
-        <f t="shared" ref="F7:F62" si="1">F6+D7+E7</f>
+        <f t="shared" ref="F7:F65" si="1">F6+D7+E7</f>
         <v>11025.640625</v>
       </c>
       <c r="G7" s="51"/>
       <c r="I7" s="45"/>
     </row>
-    <row r="8" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" ht="35.15" x14ac:dyDescent="0.45">
       <c r="B8" s="51"/>
       <c r="C8" s="49">
         <v>44348</v>
@@ -3737,7 +3693,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" ht="70.3" x14ac:dyDescent="0.45">
       <c r="B9" s="51"/>
       <c r="C9" s="49">
         <v>44378</v>
@@ -3762,7 +3718,7 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="51"/>
       <c r="C10" s="49">
         <v>44409</v>
@@ -3781,7 +3737,7 @@
       <c r="G10" s="51"/>
       <c r="J10" s="43"/>
     </row>
-    <row r="11" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" ht="52.75" x14ac:dyDescent="0.45">
       <c r="B11" s="51"/>
       <c r="C11" s="49">
         <v>44440</v>
@@ -3806,7 +3762,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" ht="52.75" x14ac:dyDescent="0.45">
       <c r="B12" s="51"/>
       <c r="C12" s="49">
         <v>44470</v>
@@ -3831,7 +3787,7 @@
         <v>1911.8040082004372</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="51"/>
       <c r="C13" s="49">
         <v>44501</v>
@@ -3849,7 +3805,7 @@
       </c>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="51"/>
       <c r="C14" s="49">
         <v>44531</v>
@@ -3867,7 +3823,7 @@
       </c>
       <c r="G14" s="51"/>
     </row>
-    <row r="15" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="51"/>
       <c r="C15" s="49">
         <v>44562</v>
@@ -3885,7 +3841,7 @@
       </c>
       <c r="G15" s="51"/>
     </row>
-    <row r="16" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="51"/>
       <c r="C16" s="49">
         <v>44593</v>
@@ -3903,7 +3859,7 @@
       </c>
       <c r="G16" s="51"/>
     </row>
-    <row r="17" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="51"/>
       <c r="C17" s="49">
         <v>44621</v>
@@ -3921,7 +3877,7 @@
       </c>
       <c r="G17" s="51"/>
     </row>
-    <row r="18" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="51"/>
       <c r="C18" s="49">
         <v>44652</v>
@@ -3939,7 +3895,7 @@
       </c>
       <c r="G18" s="51"/>
     </row>
-    <row r="19" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B19" s="51"/>
       <c r="C19" s="49">
         <v>44682</v>
@@ -3957,7 +3913,7 @@
       </c>
       <c r="G19" s="51"/>
     </row>
-    <row r="20" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B20" s="51"/>
       <c r="C20" s="49">
         <v>44713</v>
@@ -3975,7 +3931,7 @@
       </c>
       <c r="G20" s="51"/>
     </row>
-    <row r="21" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="51"/>
       <c r="C21" s="49">
         <v>44743</v>
@@ -3993,7 +3949,7 @@
       </c>
       <c r="G21" s="51"/>
     </row>
-    <row r="22" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="51"/>
       <c r="C22" s="49">
         <v>44774</v>
@@ -4011,7 +3967,7 @@
       </c>
       <c r="G22" s="51"/>
     </row>
-    <row r="23" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="51"/>
       <c r="C23" s="49">
         <v>44805</v>
@@ -4029,7 +3985,7 @@
       </c>
       <c r="G23" s="51"/>
     </row>
-    <row r="24" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="51"/>
       <c r="C24" s="49">
         <v>44835</v>
@@ -4047,7 +4003,7 @@
       </c>
       <c r="G24" s="51"/>
     </row>
-    <row r="25" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B25" s="51"/>
       <c r="C25" s="49">
         <v>44866</v>
@@ -4065,7 +4021,7 @@
       </c>
       <c r="G25" s="51"/>
     </row>
-    <row r="26" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B26" s="51"/>
       <c r="C26" s="49">
         <v>44896</v>
@@ -4083,7 +4039,7 @@
       </c>
       <c r="G26" s="51"/>
     </row>
-    <row r="27" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B27" s="51"/>
       <c r="C27" s="49">
         <v>44927</v>
@@ -4101,7 +4057,7 @@
       </c>
       <c r="G27" s="51"/>
     </row>
-    <row r="28" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B28" s="51"/>
       <c r="C28" s="49">
         <v>44958</v>
@@ -4119,7 +4075,7 @@
       </c>
       <c r="G28" s="51"/>
     </row>
-    <row r="29" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B29" s="51"/>
       <c r="C29" s="49">
         <v>44986</v>
@@ -4137,7 +4093,7 @@
       </c>
       <c r="G29" s="51"/>
     </row>
-    <row r="30" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B30" s="51"/>
       <c r="C30" s="49">
         <v>45017</v>
@@ -4155,7 +4111,7 @@
       </c>
       <c r="G30" s="51"/>
     </row>
-    <row r="31" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B31" s="51"/>
       <c r="C31" s="49">
         <v>45047</v>
@@ -4173,7 +4129,7 @@
       </c>
       <c r="G31" s="51"/>
     </row>
-    <row r="32" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B32" s="51"/>
       <c r="C32" s="49">
         <v>45078</v>
@@ -4191,7 +4147,7 @@
       </c>
       <c r="G32" s="51"/>
     </row>
-    <row r="33" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B33" s="51"/>
       <c r="C33" s="49">
         <v>45108</v>
@@ -4209,7 +4165,7 @@
       </c>
       <c r="G33" s="51"/>
     </row>
-    <row r="34" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B34" s="51"/>
       <c r="C34" s="49">
         <v>45139</v>
@@ -4227,7 +4183,7 @@
       </c>
       <c r="G34" s="51"/>
     </row>
-    <row r="35" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B35" s="51"/>
       <c r="C35" s="49">
         <v>45170</v>
@@ -4245,7 +4201,7 @@
       </c>
       <c r="G35" s="51"/>
     </row>
-    <row r="36" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B36" s="51"/>
       <c r="C36" s="49">
         <v>45200</v>
@@ -4263,7 +4219,7 @@
       </c>
       <c r="G36" s="51"/>
     </row>
-    <row r="37" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B37" s="51"/>
       <c r="C37" s="49">
         <v>45231</v>
@@ -4281,13 +4237,13 @@
       </c>
       <c r="G37" s="51"/>
     </row>
-    <row r="38" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B38" s="51"/>
       <c r="C38" s="49">
         <v>45261</v>
       </c>
       <c r="D38" s="50">
-        <f t="shared" ref="D38:D65" si="2">$J$9*F37</f>
+        <f t="shared" si="0"/>
         <v>33.402197654383656</v>
       </c>
       <c r="E38" s="50">
@@ -4299,13 +4255,13 @@
       </c>
       <c r="G38" s="51"/>
     </row>
-    <row r="39" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B39" s="51"/>
       <c r="C39" s="49">
         <v>45292</v>
       </c>
       <c r="D39" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>34.068950401451637</v>
       </c>
       <c r="E39" s="50">
@@ -4317,13 +4273,13 @@
       </c>
       <c r="G39" s="51"/>
     </row>
-    <row r="40" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B40" s="51"/>
       <c r="C40" s="49">
         <v>45323</v>
       </c>
       <c r="D40" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>34.736536589453451</v>
       </c>
       <c r="E40" s="50">
@@ -4335,13 +4291,13 @@
       </c>
       <c r="G40" s="51"/>
     </row>
-    <row r="41" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B41" s="51"/>
       <c r="C41" s="49">
         <v>45352</v>
       </c>
       <c r="D41" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>35.404957260190265</v>
       </c>
       <c r="E41" s="50">
@@ -4353,13 +4309,13 @@
       </c>
       <c r="G41" s="51"/>
     </row>
-    <row r="42" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B42" s="51"/>
       <c r="C42" s="49">
         <v>45383</v>
       </c>
       <c r="D42" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>36.074213456765506</v>
       </c>
       <c r="E42" s="50">
@@ -4371,13 +4327,13 @@
       </c>
       <c r="G42" s="51"/>
     </row>
-    <row r="43" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B43" s="51"/>
       <c r="C43" s="49">
         <v>45413</v>
       </c>
       <c r="D43" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>36.744306223586463</v>
       </c>
       <c r="E43" s="50">
@@ -4389,13 +4345,13 @@
       </c>
       <c r="G43" s="51"/>
     </row>
-    <row r="44" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B44" s="51"/>
       <c r="C44" s="49">
         <v>45444</v>
       </c>
       <c r="D44" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>37.415236606365951</v>
       </c>
       <c r="E44" s="50">
@@ -4407,13 +4363,13 @@
       </c>
       <c r="G44" s="51"/>
     </row>
-    <row r="45" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B45" s="51"/>
       <c r="C45" s="49">
         <v>45474</v>
       </c>
       <c r="D45" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>38.087005652123906</v>
       </c>
       <c r="E45" s="50">
@@ -4425,13 +4381,13 @@
       </c>
       <c r="G45" s="51"/>
     </row>
-    <row r="46" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B46" s="51"/>
       <c r="C46" s="49">
         <v>45505</v>
       </c>
       <c r="D46" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>38.759614409189055</v>
       </c>
       <c r="E46" s="50">
@@ -4443,13 +4399,13 @@
       </c>
       <c r="G46" s="51"/>
     </row>
-    <row r="47" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B47" s="51"/>
       <c r="C47" s="49">
         <v>45536</v>
       </c>
       <c r="D47" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>39.433063927200543</v>
       </c>
       <c r="E47" s="50">
@@ -4461,13 +4417,13 @@
       </c>
       <c r="G47" s="51"/>
     </row>
-    <row r="48" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B48" s="51"/>
       <c r="C48" s="49">
         <v>45566</v>
       </c>
       <c r="D48" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>40.107355257109546</v>
       </c>
       <c r="E48" s="50">
@@ -4479,13 +4435,13 @@
       </c>
       <c r="G48" s="51"/>
     </row>
-    <row r="49" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B49" s="51"/>
       <c r="C49" s="49">
         <v>45597</v>
       </c>
       <c r="D49" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>40.782489451180929</v>
       </c>
       <c r="E49" s="50">
@@ -4497,13 +4453,13 @@
       </c>
       <c r="G49" s="51"/>
     </row>
-    <row r="50" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B50" s="51"/>
       <c r="C50" s="49">
         <v>45627</v>
       </c>
       <c r="D50" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>41.458467562994905</v>
       </c>
       <c r="E50" s="50">
@@ -4515,13 +4471,13 @@
       </c>
       <c r="G50" s="51"/>
     </row>
-    <row r="51" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B51" s="51"/>
       <c r="C51" s="49">
         <v>45658</v>
       </c>
       <c r="D51" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>42.135290647448649</v>
       </c>
       <c r="E51" s="50">
@@ -4533,13 +4489,13 @@
       </c>
       <c r="G51" s="51"/>
     </row>
-    <row r="52" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B52" s="51"/>
       <c r="C52" s="49">
         <v>45689</v>
       </c>
       <c r="D52" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>42.812959760757956</v>
       </c>
       <c r="E52" s="50">
@@ -4551,13 +4507,13 @@
       </c>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B53" s="51"/>
       <c r="C53" s="49">
         <v>45717</v>
       </c>
       <c r="D53" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>43.491475960458899</v>
       </c>
       <c r="E53" s="50">
@@ -4569,13 +4525,13 @@
       </c>
       <c r="G53" s="51"/>
     </row>
-    <row r="54" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B54" s="51"/>
       <c r="C54" s="49">
         <v>45748</v>
       </c>
       <c r="D54" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>44.170840305409477</v>
       </c>
       <c r="E54" s="50">
@@ -4587,13 +4543,13 @@
       </c>
       <c r="G54" s="51"/>
     </row>
-    <row r="55" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B55" s="51"/>
       <c r="C55" s="49">
         <v>45778</v>
       </c>
       <c r="D55" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>44.851053855791235</v>
       </c>
       <c r="E55" s="50">
@@ -4605,13 +4561,13 @@
       </c>
       <c r="G55" s="51"/>
     </row>
-    <row r="56" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B56" s="51"/>
       <c r="C56" s="49">
         <v>45809</v>
       </c>
       <c r="D56" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>45.532117673110967</v>
       </c>
       <c r="E56" s="50">
@@ -4623,13 +4579,13 @@
       </c>
       <c r="G56" s="51"/>
     </row>
-    <row r="57" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B57" s="51"/>
       <c r="C57" s="49">
         <v>45839</v>
       </c>
       <c r="D57" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>46.214032820202355</v>
       </c>
       <c r="E57" s="50">
@@ -4641,13 +4597,13 @@
       </c>
       <c r="G57" s="51"/>
     </row>
-    <row r="58" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B58" s="51"/>
       <c r="C58" s="49">
         <v>45870</v>
       </c>
       <c r="D58" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>46.896800361227605</v>
       </c>
       <c r="E58" s="50">
@@ -4659,13 +4615,13 @@
       </c>
       <c r="G58" s="51"/>
     </row>
-    <row r="59" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B59" s="51"/>
       <c r="C59" s="49">
         <v>45901</v>
       </c>
       <c r="D59" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>47.580421361679136</v>
       </c>
       <c r="E59" s="50">
@@ -4677,13 +4633,13 @@
       </c>
       <c r="G59" s="51"/>
     </row>
-    <row r="60" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B60" s="51"/>
       <c r="C60" s="49">
         <v>45931</v>
       </c>
       <c r="D60" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>48.264896888381237</v>
       </c>
       <c r="E60" s="50">
@@ -4695,13 +4651,13 @@
       </c>
       <c r="G60" s="51"/>
     </row>
-    <row r="61" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B61" s="51"/>
       <c r="C61" s="49">
         <v>45962</v>
       </c>
       <c r="D61" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>48.95022800949171</v>
       </c>
       <c r="E61" s="50">
@@ -4713,13 +4669,13 @@
       </c>
       <c r="G61" s="51"/>
     </row>
-    <row r="62" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B62" s="51"/>
       <c r="C62" s="49">
         <v>45992</v>
       </c>
       <c r="D62" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>49.636415794503577</v>
       </c>
       <c r="E62" s="50">
@@ -4731,56 +4687,56 @@
       </c>
       <c r="G62" s="51"/>
     </row>
-    <row r="63" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B63" s="51"/>
       <c r="C63" s="49">
         <v>46023</v>
       </c>
       <c r="D63" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>50.323461314246707</v>
       </c>
       <c r="E63" s="50">
         <v>500</v>
       </c>
       <c r="F63" s="50">
-        <f t="shared" ref="F63:F65" si="3">F62+D63+E63</f>
+        <f t="shared" si="1"/>
         <v>40809.092512711613</v>
       </c>
       <c r="G63" s="51"/>
     </row>
-    <row r="64" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B64" s="51"/>
       <c r="C64" s="49">
         <v>46054</v>
       </c>
       <c r="D64" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>51.011365640889515</v>
       </c>
       <c r="E64" s="50">
         <v>500</v>
       </c>
       <c r="F64" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>41360.1038783525</v>
       </c>
       <c r="G64" s="51"/>
     </row>
-    <row r="65" spans="2:7" ht="40" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B65" s="51"/>
       <c r="C65" s="49">
         <v>46082</v>
       </c>
       <c r="D65" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>51.700129847940623</v>
       </c>
       <c r="E65" s="50">
         <v>500</v>
       </c>
       <c r="F65" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>41911.804008200437</v>
       </c>
       <c r="G65" s="51"/>
@@ -4808,14 +4764,42 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5115,36 +5099,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AB306A1-AFF6-40CB-BF3D-1EF22BB7168E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5165,26 +5140,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
fix: update family budget spreadsheet with changes
Updated the "Family budget monthly.xlsx" file to ensure its contents are accurate and align with the latest requirements. This maintains the reliability of the budgeting data.
</commit_message>
<xml_diff>
--- a/spreadsheets/Family budget monthly.xlsx
+++ b/spreadsheets/Family budget monthly.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35C3E1D-0E4D-42AD-BCA1-842F43FAA3A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A629F-5D0F-40D9-B2DF-8C1D720FAD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1886" yWindow="1886" windowWidth="16628" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly budget report" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Interest" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses" hidden="1">TBL_MonthlyExpenses[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses1" hidden="1">TBL_MonthlyExpenses[]</definedName>
     <definedName name="List_ExpenseCategories">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Monthly expenses'!$2:$4</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="TBL_MonthlyExpenses" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TEMP.xlsxTBL_MonthlyExpenses1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1851,8 +1851,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2074,10 +2074,7 @@
       <c r="C11" s="35"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="24">
-        <f>SUM(F7:F10)</f>
-        <v>200</v>
-      </c>
+      <c r="F11" s="24"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -2210,10 +2207,7 @@
       <c r="C18" s="38"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
-      <c r="F18" s="27">
-        <f>SUM(F15:F17)</f>
-        <v>100</v>
-      </c>
+      <c r="F18" s="27"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -4771,35 +4765,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5099,27 +5064,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AB306A1-AFF6-40CB-BF3D-1EF22BB7168E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5140,6 +5114,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67610313-8E8D-4F0A-9821-51B850A6E13F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{082E568A-D275-4349-BB4E-0AE14394E51D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>